<commit_message>
changed rejection in improvement
</commit_message>
<xml_diff>
--- a/data/comparazioni.xlsx
+++ b/data/comparazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/livia_simoncini_alumni_uniroma2_eu/Documents/Corsi/Attivi/PMCSN/Progetto/PMCSN_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="233" documentId="8_{E9DA16B5-D2F2-4171-AC27-5E17BCEA9C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5316A325-B8F2-42D7-A0A6-68198A93B0A5}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="8_{E9DA16B5-D2F2-4171-AC27-5E17BCEA9C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FDBA8AE-277B-4C2D-ABA1-F2D53CB5A8F4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA442C77-0058-4E5D-AB51-BAFF26F9EAEA}"/>
   </bookViews>
@@ -16,15 +16,6 @@
     <sheet name="Identical VS Compatible" sheetId="3" r:id="rId1"/>
     <sheet name="Compatible VS Incompatible" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Compatible VS Incompatible'!$D$3:$D$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Compatible VS Incompatible'!$E$3:$E$10</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Compatible VS Incompatible'!$D$2:$E$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Compatible VS Incompatible'!$D$3:$D$10</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Compatible VS Incompatible'!$E$3:$E$10</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Compatible VS Incompatible'!$F$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Compatible VS Incompatible'!$F$3:$F$10</definedName>
-  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="45">
   <si>
     <t>Average number of patients in the activation center</t>
   </si>
@@ -170,6 +161,18 @@
   <si>
     <t>Average number of patients activated</t>
   </si>
+  <si>
+    <t>Average number of transplants</t>
+  </si>
+  <si>
+    <t>Average number of successful transplants</t>
+  </si>
+  <si>
+    <t>Average number of rejected transplants</t>
+  </si>
+  <si>
+    <t>Average number of organ outdatings</t>
+  </si>
 </sst>
 </file>
 
@@ -189,7 +192,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +208,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -353,6 +362,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -365,43 +380,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -416,13 +422,45 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -743,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BCF3B6-51B1-48FA-984F-EC30D107B6D0}">
   <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115:XFD122"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -758,34 +796,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="30"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1866,41 +1904,41 @@
       <c r="G90" s="4"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="19"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="21"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="25"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="25" t="s">
+      <c r="A92" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="27" t="s">
+      <c r="C92" s="17"/>
+      <c r="D92" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E92" s="28"/>
-      <c r="F92" s="29" t="s">
+      <c r="E92" s="27"/>
+      <c r="F92" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G92" s="30"/>
+      <c r="G92" s="29"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C93" s="16"/>
+      <c r="C93" s="21"/>
       <c r="D93" s="7"/>
       <c r="E93" s="6"/>
       <c r="F93" s="7"/>
@@ -1908,10 +1946,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
-      <c r="B94" s="10" t="s">
+      <c r="B94" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="11"/>
+      <c r="C94" s="13"/>
       <c r="D94" s="3"/>
       <c r="E94" s="5"/>
       <c r="F94" s="3"/>
@@ -1919,10 +1957,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
-      <c r="B95" s="10" t="s">
+      <c r="B95" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C95" s="11"/>
+      <c r="C95" s="13"/>
       <c r="D95" s="3"/>
       <c r="E95" s="5"/>
       <c r="F95" s="3"/>
@@ -1930,10 +1968,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
-      <c r="B96" s="10" t="s">
+      <c r="B96" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="11"/>
+      <c r="C96" s="13"/>
       <c r="D96" s="3"/>
       <c r="E96" s="5"/>
       <c r="F96" s="3"/>
@@ -1943,10 +1981,10 @@
       <c r="A97" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B97" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="11"/>
+      <c r="C97" s="13"/>
       <c r="D97" s="3"/>
       <c r="E97" s="5"/>
       <c r="F97" s="3"/>
@@ -1954,10 +1992,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C98" s="11"/>
+      <c r="C98" s="13"/>
       <c r="D98" s="3"/>
       <c r="E98" s="5"/>
       <c r="F98" s="3"/>
@@ -1965,10 +2003,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
-      <c r="B99" s="10" t="s">
+      <c r="B99" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="11"/>
+      <c r="C99" s="13"/>
       <c r="D99" s="3"/>
       <c r="E99" s="5"/>
       <c r="F99" s="3"/>
@@ -1976,10 +2014,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
-      <c r="B100" s="10" t="s">
+      <c r="B100" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C100" s="11"/>
+      <c r="C100" s="13"/>
       <c r="D100" s="3"/>
       <c r="E100" s="5"/>
       <c r="F100" s="3"/>
@@ -1987,12 +2025,12 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B101" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C101" s="11"/>
+      <c r="C101" s="13"/>
       <c r="D101" s="3"/>
       <c r="E101" s="5"/>
       <c r="F101" s="3"/>
@@ -2000,10 +2038,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
-      <c r="B102" s="10" t="s">
+      <c r="B102" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C102" s="11"/>
+      <c r="C102" s="13"/>
       <c r="D102" s="3"/>
       <c r="E102" s="5"/>
       <c r="F102" s="3"/>
@@ -2011,10 +2049,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="3"/>
-      <c r="B103" s="10" t="s">
+      <c r="B103" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="11"/>
+      <c r="C103" s="13"/>
       <c r="D103" s="3"/>
       <c r="E103" s="5"/>
       <c r="F103" s="3"/>
@@ -2022,10 +2060,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
-      <c r="B104" s="10" t="s">
+      <c r="B104" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="11"/>
+      <c r="C104" s="13"/>
       <c r="D104" s="3"/>
       <c r="E104" s="5"/>
       <c r="F104" s="3"/>
@@ -2035,10 +2073,10 @@
       <c r="A105" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B105" s="10" t="s">
+      <c r="B105" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="11"/>
+      <c r="C105" s="13"/>
       <c r="D105" s="3"/>
       <c r="E105" s="5"/>
       <c r="F105" s="3"/>
@@ -2046,10 +2084,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
-      <c r="B106" s="10" t="s">
+      <c r="B106" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C106" s="11"/>
+      <c r="C106" s="13"/>
       <c r="D106" s="3"/>
       <c r="E106" s="5"/>
       <c r="F106" s="3"/>
@@ -2057,10 +2095,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
-      <c r="B107" s="10" t="s">
+      <c r="B107" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C107" s="11"/>
+      <c r="C107" s="13"/>
       <c r="D107" s="3"/>
       <c r="E107" s="5"/>
       <c r="F107" s="3"/>
@@ -2068,10 +2106,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
-      <c r="B108" s="10" t="s">
+      <c r="B108" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C108" s="11"/>
+      <c r="C108" s="13"/>
       <c r="D108" s="3"/>
       <c r="E108" s="5"/>
       <c r="F108" s="3"/>
@@ -2081,10 +2119,10 @@
       <c r="A109" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B109" s="10" t="s">
+      <c r="B109" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C109" s="11"/>
+      <c r="C109" s="13"/>
       <c r="D109" s="3"/>
       <c r="E109" s="5"/>
       <c r="F109" s="3"/>
@@ -2092,10 +2130,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
-      <c r="B110" s="10" t="s">
+      <c r="B110" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C110" s="11"/>
+      <c r="C110" s="13"/>
       <c r="D110" s="3"/>
       <c r="E110" s="5"/>
       <c r="F110" s="3"/>
@@ -2103,10 +2141,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
-      <c r="B111" s="10" t="s">
+      <c r="B111" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C111" s="11"/>
+      <c r="C111" s="13"/>
       <c r="D111" s="3"/>
       <c r="E111" s="5"/>
       <c r="F111" s="3"/>
@@ -2114,44 +2152,44 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
-      <c r="B112" s="12" t="s">
+      <c r="B112" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C112" s="13"/>
+      <c r="C112" s="15"/>
       <c r="D112" s="2"/>
       <c r="E112" s="4"/>
       <c r="F112" s="2"/>
       <c r="G112" s="4"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B113" s="20"/>
-      <c r="C113" s="20"/>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="21"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="25"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="25" t="s">
+      <c r="A114" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B114" s="25" t="s">
+      <c r="B114" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C114" s="26" t="s">
+      <c r="C114" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D114" s="27" t="s">
+      <c r="D114" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E114" s="28"/>
-      <c r="F114" s="29" t="s">
+      <c r="E114" s="27"/>
+      <c r="F114" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G114" s="30"/>
+      <c r="G114" s="29"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
@@ -2557,41 +2595,41 @@
       <c r="G147" s="4"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="18" t="s">
+      <c r="A148" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B148" s="19"/>
-      <c r="C148" s="19"/>
-      <c r="D148" s="20"/>
-      <c r="E148" s="20"/>
-      <c r="F148" s="19"/>
-      <c r="G148" s="21"/>
+      <c r="B148" s="24"/>
+      <c r="C148" s="24"/>
+      <c r="D148" s="23"/>
+      <c r="E148" s="23"/>
+      <c r="F148" s="24"/>
+      <c r="G148" s="25"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="25" t="s">
+      <c r="A149" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B149" s="31" t="s">
+      <c r="B149" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C149" s="32"/>
-      <c r="D149" s="29" t="s">
+      <c r="C149" s="17"/>
+      <c r="D149" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E149" s="30"/>
-      <c r="F149" s="29" t="s">
+      <c r="E149" s="29"/>
+      <c r="F149" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G149" s="30"/>
+      <c r="G149" s="29"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B150" s="15" t="s">
+      <c r="B150" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C150" s="17"/>
+      <c r="C150" s="20"/>
       <c r="D150" s="7"/>
       <c r="E150" s="6"/>
       <c r="F150" s="7"/>
@@ -2599,10 +2637,10 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
-      <c r="B151" s="10" t="s">
+      <c r="B151" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C151" s="14"/>
+      <c r="C151" s="18"/>
       <c r="D151" s="3"/>
       <c r="E151" s="5"/>
       <c r="F151" s="3"/>
@@ -2610,10 +2648,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="3"/>
-      <c r="B152" s="10" t="s">
+      <c r="B152" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C152" s="14"/>
+      <c r="C152" s="18"/>
       <c r="D152" s="3"/>
       <c r="E152" s="5"/>
       <c r="F152" s="3"/>
@@ -2621,10 +2659,10 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
-      <c r="B153" s="10" t="s">
+      <c r="B153" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C153" s="14"/>
+      <c r="C153" s="18"/>
       <c r="D153" s="3"/>
       <c r="E153" s="5"/>
       <c r="F153" s="3"/>
@@ -2634,10 +2672,10 @@
       <c r="A154" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B154" s="10" t="s">
+      <c r="B154" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C154" s="14"/>
+      <c r="C154" s="18"/>
       <c r="D154" s="3"/>
       <c r="E154" s="5"/>
       <c r="F154" s="3"/>
@@ -2645,10 +2683,10 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
-      <c r="B155" s="10" t="s">
+      <c r="B155" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C155" s="14"/>
+      <c r="C155" s="18"/>
       <c r="D155" s="3"/>
       <c r="E155" s="5"/>
       <c r="F155" s="3"/>
@@ -2656,10 +2694,10 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
-      <c r="B156" s="10" t="s">
+      <c r="B156" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C156" s="14"/>
+      <c r="C156" s="18"/>
       <c r="D156" s="3"/>
       <c r="E156" s="5"/>
       <c r="F156" s="3"/>
@@ -2667,10 +2705,10 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
-      <c r="B157" s="10" t="s">
+      <c r="B157" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C157" s="14"/>
+      <c r="C157" s="18"/>
       <c r="D157" s="3"/>
       <c r="E157" s="5"/>
       <c r="F157" s="3"/>
@@ -2680,10 +2718,10 @@
       <c r="A158" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B158" s="10" t="s">
+      <c r="B158" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C158" s="14"/>
+      <c r="C158" s="18"/>
       <c r="D158" s="3"/>
       <c r="E158" s="5"/>
       <c r="F158" s="3"/>
@@ -2691,10 +2729,10 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="3"/>
-      <c r="B159" s="10" t="s">
+      <c r="B159" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C159" s="14"/>
+      <c r="C159" s="18"/>
       <c r="D159" s="3"/>
       <c r="E159" s="5"/>
       <c r="F159" s="3"/>
@@ -2702,10 +2740,10 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="3"/>
-      <c r="B160" s="10" t="s">
+      <c r="B160" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C160" s="14"/>
+      <c r="C160" s="18"/>
       <c r="D160" s="3"/>
       <c r="E160" s="5"/>
       <c r="F160" s="3"/>
@@ -2713,10 +2751,10 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="3"/>
-      <c r="B161" s="10" t="s">
+      <c r="B161" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C161" s="14"/>
+      <c r="C161" s="18"/>
       <c r="D161" s="3"/>
       <c r="E161" s="5"/>
       <c r="F161" s="3"/>
@@ -2726,10 +2764,10 @@
       <c r="A162" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B162" s="10" t="s">
+      <c r="B162" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C162" s="14"/>
+      <c r="C162" s="18"/>
       <c r="D162" s="3"/>
       <c r="E162" s="5"/>
       <c r="F162" s="3"/>
@@ -2737,10 +2775,10 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="3"/>
-      <c r="B163" s="10" t="s">
+      <c r="B163" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C163" s="14"/>
+      <c r="C163" s="18"/>
       <c r="D163" s="3"/>
       <c r="E163" s="5"/>
       <c r="F163" s="3"/>
@@ -2748,10 +2786,10 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
-      <c r="B164" s="10" t="s">
+      <c r="B164" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C164" s="14"/>
+      <c r="C164" s="18"/>
       <c r="D164" s="3"/>
       <c r="E164" s="5"/>
       <c r="F164" s="3"/>
@@ -2759,10 +2797,10 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
-      <c r="B165" s="10" t="s">
+      <c r="B165" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C165" s="14"/>
+      <c r="C165" s="18"/>
       <c r="D165" s="3"/>
       <c r="E165" s="5"/>
       <c r="F165" s="3"/>
@@ -2787,34 +2825,34 @@
     <mergeCell ref="A91:G91"/>
     <mergeCell ref="D92:E92"/>
     <mergeCell ref="F92:G92"/>
-    <mergeCell ref="B159:C159"/>
     <mergeCell ref="A113:G113"/>
     <mergeCell ref="D114:E114"/>
     <mergeCell ref="F114:G114"/>
     <mergeCell ref="A148:G148"/>
     <mergeCell ref="D149:E149"/>
     <mergeCell ref="F149:G149"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B149:C149"/>
     <mergeCell ref="B93:C93"/>
     <mergeCell ref="B94:C94"/>
     <mergeCell ref="B95:C95"/>
     <mergeCell ref="B96:C96"/>
     <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B164:C164"/>
     <mergeCell ref="B165:C165"/>
     <mergeCell ref="B150:C150"/>
     <mergeCell ref="B151:C151"/>
     <mergeCell ref="B152:C152"/>
     <mergeCell ref="B153:C153"/>
     <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B157:C157"/>
     <mergeCell ref="B110:C110"/>
     <mergeCell ref="B111:C111"/>
     <mergeCell ref="B112:C112"/>
@@ -2840,8 +2878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2317ED-57BA-4FAE-A3A8-363C38207229}">
   <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I122" sqref="I122"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150:G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2855,34 +2893,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="29"/>
+      <c r="F2" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="30"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -2895,16 +2933,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="3">
-        <v>16.412697999999999</v>
+        <v>16.603175</v>
       </c>
       <c r="E3" s="5">
-        <v>1.236802</v>
+        <v>1.137626</v>
       </c>
       <c r="F3" s="3">
-        <v>19.174603000000001</v>
+        <v>17.761904999999999</v>
       </c>
       <c r="G3" s="5">
-        <v>1.5033019999999999</v>
+        <v>1.3851309999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2914,16 +2952,16 @@
         <v>4</v>
       </c>
       <c r="D4" s="3">
-        <v>12448.730159000001</v>
+        <v>12453.269840999999</v>
       </c>
       <c r="E4" s="5">
-        <v>22.895330999999999</v>
+        <v>24.070218000000001</v>
       </c>
       <c r="F4" s="3">
-        <v>12906.571429</v>
+        <v>12912.714286</v>
       </c>
       <c r="G4" s="5">
-        <v>24.189416000000001</v>
+        <v>22.892257000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2935,16 +2973,16 @@
         <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>8.8253970000000006</v>
+        <v>9.6031750000000002</v>
       </c>
       <c r="E5" s="5">
-        <v>0.77892700000000004</v>
+        <v>0.86244500000000002</v>
       </c>
       <c r="F5" s="3">
-        <v>9.9206350000000008</v>
+        <v>9.7619050000000005</v>
       </c>
       <c r="G5" s="5">
-        <v>1.018799</v>
+        <v>0.83247700000000002</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2954,16 +2992,16 @@
         <v>4</v>
       </c>
       <c r="D6" s="3">
-        <v>8190.1587300000001</v>
+        <v>8195.793651</v>
       </c>
       <c r="E6" s="5">
-        <v>20.989345</v>
+        <v>20.996456999999999</v>
       </c>
       <c r="F6" s="3">
-        <v>8506.5873019999999</v>
+        <v>8503.5555559999993</v>
       </c>
       <c r="G6" s="5">
-        <v>24.276123999999999</v>
+        <v>22.007697</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2975,16 +3013,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="3">
-        <v>5.0634920000000001</v>
+        <v>5.4444439999999998</v>
       </c>
       <c r="E7" s="5">
-        <v>0.73616400000000004</v>
+        <v>0.64570499999999997</v>
       </c>
       <c r="F7" s="3">
-        <v>5.6666670000000003</v>
+        <v>5.5873020000000002</v>
       </c>
       <c r="G7" s="5">
-        <v>0.65078999999999998</v>
+        <v>0.62943000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2994,16 +3032,16 @@
         <v>4</v>
       </c>
       <c r="D8" s="3">
-        <v>3779.9841270000002</v>
+        <v>3782</v>
       </c>
       <c r="E8" s="5">
-        <v>17.619723</v>
+        <v>18.983803999999999</v>
       </c>
       <c r="F8" s="3">
-        <v>3925.666667</v>
+        <v>3927.1428569999998</v>
       </c>
       <c r="G8" s="5">
-        <v>18.133133999999998</v>
+        <v>17.599875999999998</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3018,13 +3056,13 @@
         <v>1.730159</v>
       </c>
       <c r="E9" s="5">
-        <v>0.39226800000000001</v>
+        <v>0.387017</v>
       </c>
       <c r="F9" s="3">
-        <v>1.730159</v>
+        <v>1.9206350000000001</v>
       </c>
       <c r="G9" s="5">
-        <v>0.35387800000000003</v>
+        <v>0.39511400000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3034,16 +3072,16 @@
         <v>4</v>
       </c>
       <c r="D10" s="3">
-        <v>989.031746</v>
+        <v>985.65079400000002</v>
       </c>
       <c r="E10" s="5">
-        <v>8.6341710000000003</v>
+        <v>6.6886999999999999</v>
       </c>
       <c r="F10" s="3">
-        <v>992.31745999999998</v>
+        <v>988.36507900000004</v>
       </c>
       <c r="G10" s="5">
-        <v>8.0721380000000007</v>
+        <v>8.7080649999999995</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3076,16 +3114,16 @@
         <v>4</v>
       </c>
       <c r="D12" s="3">
-        <v>935.38095199999998</v>
+        <v>932.88888899999995</v>
       </c>
       <c r="E12" s="5">
-        <v>7.8287649999999998</v>
+        <v>7.2597379999999996</v>
       </c>
       <c r="F12" s="3">
-        <v>933.66666699999996</v>
+        <v>938.77777800000001</v>
       </c>
       <c r="G12" s="5">
-        <v>7.0582339999999997</v>
+        <v>8.6933849999999993</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3116,16 +3154,16 @@
         <v>4</v>
       </c>
       <c r="D14" s="3">
-        <v>472.79365100000001</v>
+        <v>469.39682499999998</v>
       </c>
       <c r="E14" s="5">
-        <v>5.4340190000000002</v>
+        <v>5.6524140000000003</v>
       </c>
       <c r="F14" s="3">
-        <v>475.63492100000002</v>
+        <v>468.76190500000001</v>
       </c>
       <c r="G14" s="5">
-        <v>5.4106509999999997</v>
+        <v>6.031396</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3156,16 +3194,16 @@
         <v>4</v>
       </c>
       <c r="D16" s="3">
-        <v>285.80952400000001</v>
+        <v>285.22222199999999</v>
       </c>
       <c r="E16" s="5">
-        <v>4.2342680000000001</v>
+        <v>4.7695509999999999</v>
       </c>
       <c r="F16" s="3">
-        <v>282.60317500000002</v>
+        <v>282.33333299999998</v>
       </c>
       <c r="G16" s="5">
-        <v>3.9169119999999999</v>
+        <v>4.1849699999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3196,16 +3234,16 @@
         <v>4</v>
       </c>
       <c r="D18" s="3">
-        <v>40.952381000000003</v>
+        <v>42.507936999999998</v>
       </c>
       <c r="E18" s="5">
-        <v>1.643664</v>
+        <v>1.5727</v>
       </c>
       <c r="F18" s="3">
-        <v>41.666666999999997</v>
+        <v>41.809524000000003</v>
       </c>
       <c r="G18" s="5">
-        <v>1.757115</v>
+        <v>1.725897</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -3219,10 +3257,10 @@
         <v>5</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>4.7619000000000002E-2</v>
       </c>
       <c r="E19" s="5">
-        <v>0</v>
+        <v>5.4064000000000001E-2</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
@@ -3238,16 +3276,16 @@
         <v>4</v>
       </c>
       <c r="D20" s="3">
-        <v>1441.1111109999999</v>
+        <v>1439.68254</v>
       </c>
       <c r="E20" s="5">
-        <v>9.3669589999999996</v>
+        <v>9.047034</v>
       </c>
       <c r="F20" s="3">
-        <v>1440.31746</v>
+        <v>1442.126984</v>
       </c>
       <c r="G20" s="5">
-        <v>10.086131999999999</v>
+        <v>9.5331709999999994</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3278,16 +3316,16 @@
         <v>4</v>
       </c>
       <c r="D22" s="3">
-        <v>817.39682500000004</v>
+        <v>819.936508</v>
       </c>
       <c r="E22" s="5">
-        <v>8.8717299999999994</v>
+        <v>7.9165359999999998</v>
       </c>
       <c r="F22" s="3">
-        <v>819.41269799999998</v>
+        <v>815.04761900000005</v>
       </c>
       <c r="G22" s="5">
-        <v>7.3093849999999998</v>
+        <v>7.1377100000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3318,16 +3356,16 @@
         <v>4</v>
       </c>
       <c r="D24" s="3">
-        <v>429.23809499999999</v>
+        <v>429.90476200000001</v>
       </c>
       <c r="E24" s="5">
-        <v>4.718502</v>
+        <v>4.5977110000000003</v>
       </c>
       <c r="F24" s="3">
-        <v>430.936508</v>
+        <v>430.23809499999999</v>
       </c>
       <c r="G24" s="5">
-        <v>5.8811390000000001</v>
+        <v>4.8430410000000004</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -3358,16 +3396,16 @@
         <v>4</v>
       </c>
       <c r="D26" s="3">
-        <v>72.412698000000006</v>
+        <v>74.444444000000004</v>
       </c>
       <c r="E26" s="5">
-        <v>2.352827</v>
+        <v>2.133051</v>
       </c>
       <c r="F26" s="3">
-        <v>75.317459999999997</v>
+        <v>76.460317000000003</v>
       </c>
       <c r="G26" s="5">
-        <v>2.0323799999999999</v>
+        <v>2.0464250000000002</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -3396,11 +3434,11 @@
         <v>4</v>
       </c>
       <c r="D28" s="3">
-        <v>211479</v>
+        <v>210532</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="3">
-        <v>231804</v>
+        <v>231842</v>
       </c>
       <c r="G28" s="5"/>
     </row>
@@ -3428,11 +3466,11 @@
         <v>4</v>
       </c>
       <c r="D30" s="3">
-        <v>140313</v>
+        <v>139715</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="3">
-        <v>154090</v>
+        <v>154187</v>
       </c>
       <c r="G30" s="5"/>
     </row>
@@ -3460,11 +3498,11 @@
         <v>4</v>
       </c>
       <c r="D32" s="3">
-        <v>64061</v>
+        <v>63917</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="3">
-        <v>70311</v>
+        <v>70534</v>
       </c>
       <c r="G32" s="5"/>
     </row>
@@ -3492,11 +3530,11 @@
         <v>4</v>
       </c>
       <c r="D34" s="3">
-        <v>15</v>
+        <v>1572</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="3">
-        <v>18034</v>
+        <v>17994</v>
       </c>
       <c r="G34" s="5"/>
     </row>
@@ -3511,16 +3549,16 @@
         <v>5</v>
       </c>
       <c r="D35" s="3">
-        <v>21.881888</v>
+        <v>21.603562</v>
       </c>
       <c r="E35" s="5">
-        <v>0.27078600000000003</v>
+        <v>0.25826100000000002</v>
       </c>
       <c r="F35" s="3">
-        <v>18.437573</v>
+        <v>20.263798999999999</v>
       </c>
       <c r="G35" s="5">
-        <v>0.27803800000000001</v>
+        <v>0.22117300000000001</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -3530,16 +3568,16 @@
         <v>4</v>
       </c>
       <c r="D36" s="3">
-        <v>2.9335E-2</v>
+        <v>2.9323999999999999E-2</v>
       </c>
       <c r="E36" s="5">
-        <v>5.0000000000000004E-6</v>
+        <v>6.9999999999999999E-6</v>
       </c>
       <c r="F36" s="3">
-        <v>2.8317999999999999E-2</v>
+        <v>2.8302999999999998E-2</v>
       </c>
       <c r="G36" s="5">
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -3551,16 +3589,16 @@
         <v>5</v>
       </c>
       <c r="D37" s="3">
-        <v>41.860581000000003</v>
+        <v>39.742883999999997</v>
       </c>
       <c r="E37" s="5">
-        <v>0.47930200000000001</v>
+        <v>0.54322199999999998</v>
       </c>
       <c r="F37" s="3">
-        <v>37.069198999999998</v>
+        <v>36.118878000000002</v>
       </c>
       <c r="G37" s="5">
-        <v>0.40981400000000001</v>
+        <v>0.49256</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -3570,16 +3608,16 @@
         <v>4</v>
       </c>
       <c r="D38" s="3">
-        <v>4.4631999999999998E-2</v>
+        <v>4.4595000000000003E-2</v>
       </c>
       <c r="E38" s="5">
-        <v>3.8000000000000002E-5</v>
+        <v>3.3000000000000003E-5</v>
       </c>
       <c r="F38" s="3">
-        <v>4.3043999999999999E-2</v>
+        <v>4.3024E-2</v>
       </c>
       <c r="G38" s="5">
-        <v>6.6000000000000005E-5</v>
+        <v>4.8999999999999998E-5</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -3591,16 +3629,16 @@
         <v>5</v>
       </c>
       <c r="D39" s="3">
-        <v>83.786254</v>
+        <v>80.481656999999998</v>
       </c>
       <c r="E39" s="5">
-        <v>10.334777000000001</v>
+        <v>10.729193</v>
       </c>
       <c r="F39" s="3">
-        <v>62.942321</v>
+        <v>72.993915999999999</v>
       </c>
       <c r="G39" s="5">
-        <v>1.541863</v>
+        <v>10.319675</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -3610,16 +3648,16 @@
         <v>4</v>
       </c>
       <c r="D40" s="3">
-        <v>9.6096000000000001E-2</v>
+        <v>9.6160999999999996E-2</v>
       </c>
       <c r="E40" s="5">
-        <v>1.36E-4</v>
+        <v>1.03E-4</v>
       </c>
       <c r="F40" s="3">
-        <v>9.2629000000000003E-2</v>
+        <v>9.2627000000000001E-2</v>
       </c>
       <c r="G40" s="5">
-        <v>9.5000000000000005E-5</v>
+        <v>8.7000000000000001E-5</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -3631,16 +3669,16 @@
         <v>5</v>
       </c>
       <c r="D41" s="3">
-        <v>184.104806</v>
+        <v>188.720493</v>
       </c>
       <c r="E41" s="5">
-        <v>9.3703710000000004</v>
+        <v>7.8930550000000004</v>
       </c>
       <c r="F41" s="3">
-        <v>191.97196400000001</v>
+        <v>173.91171800000001</v>
       </c>
       <c r="G41" s="5">
-        <v>7.5397020000000001</v>
+        <v>5.3002500000000001</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -3650,16 +3688,16 @@
         <v>4</v>
       </c>
       <c r="D42" s="3">
-        <v>0.37067800000000001</v>
+        <v>0.37013000000000001</v>
       </c>
       <c r="E42" s="5">
-        <v>8.2600000000000002E-4</v>
+        <v>5.2400000000000005E-4</v>
       </c>
       <c r="F42" s="3">
-        <v>0.36716500000000002</v>
+        <v>0.37127399999999999</v>
       </c>
       <c r="G42" s="5">
-        <v>4.3899999999999999E-4</v>
+        <v>6.8900000000000005E-4</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -3673,16 +3711,16 @@
         <v>5</v>
       </c>
       <c r="D43" s="3">
-        <v>2.32E-4</v>
+        <v>4.6799999999999999E-4</v>
       </c>
       <c r="E43" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="F43" s="3">
-        <v>7.3999999999999996E-5</v>
+        <v>6.3E-5</v>
       </c>
       <c r="G43" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -3692,16 +3730,16 @@
         <v>4</v>
       </c>
       <c r="D44" s="3">
-        <v>2841.4266389999998</v>
+        <v>2823.3028920000002</v>
       </c>
       <c r="E44" s="5">
-        <v>409.66005699999999</v>
+        <v>406.83753200000001</v>
       </c>
       <c r="F44" s="3">
-        <v>3033.5626229999998</v>
+        <v>3036.0826240000001</v>
       </c>
       <c r="G44" s="5">
-        <v>439.16756600000002</v>
+        <v>439.83436899999998</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -3713,16 +3751,16 @@
         <v>5</v>
       </c>
       <c r="D45" s="3">
-        <v>1.01E-4</v>
+        <v>2.32E-4</v>
       </c>
       <c r="E45" s="5">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="F45" s="3">
+        <v>5.3999999999999998E-5</v>
+      </c>
+      <c r="G45" s="5">
         <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="F45" s="3">
-        <v>4.8999999999999998E-5</v>
-      </c>
-      <c r="G45" s="5">
-        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -3732,16 +3770,16 @@
         <v>4</v>
       </c>
       <c r="D46" s="3">
-        <v>2702.4383670000002</v>
+        <v>2696.1794329999998</v>
       </c>
       <c r="E46" s="5">
-        <v>391.28761300000002</v>
+        <v>389.06897800000002</v>
       </c>
       <c r="F46" s="3">
-        <v>2911.4701909999999</v>
+        <v>2901.333905</v>
       </c>
       <c r="G46" s="5">
-        <v>420.69536099999999</v>
+        <v>420.20657899999998</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -3753,16 +3791,16 @@
         <v>5</v>
       </c>
       <c r="D47" s="3">
-        <v>1.7699999999999999E-4</v>
+        <v>3.3799999999999998E-4</v>
       </c>
       <c r="E47" s="5">
-        <v>7.9999999999999996E-6</v>
+        <v>2.0999999999999999E-5</v>
       </c>
       <c r="F47" s="3">
-        <v>6.7999999999999999E-5</v>
+        <v>6.4999999999999994E-5</v>
       </c>
       <c r="G47" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>3.0000000000000001E-6</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -3772,16 +3810,16 @@
         <v>4</v>
       </c>
       <c r="D48" s="3">
-        <v>2803.8567109999999</v>
+        <v>2799.533144</v>
       </c>
       <c r="E48" s="5">
-        <v>405.61908099999999</v>
+        <v>403.90964300000002</v>
       </c>
       <c r="F48" s="3">
-        <v>3001.8789299999999</v>
+        <v>3002.307742</v>
       </c>
       <c r="G48" s="5">
-        <v>435.380357</v>
+        <v>434.755246</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -3793,16 +3831,16 @@
         <v>5</v>
       </c>
       <c r="D49" s="3">
-        <v>1.08E-4</v>
+        <v>2.63E-4</v>
       </c>
       <c r="E49" s="5">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="G49" s="5">
         <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="F49" s="3">
-        <v>8.2000000000000001E-5</v>
-      </c>
-      <c r="G49" s="5">
-        <v>3.9999999999999998E-6</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -3812,16 +3850,16 @@
         <v>4</v>
       </c>
       <c r="D50" s="3">
-        <v>7.0227339999999998</v>
+        <v>124.16471199999999</v>
       </c>
       <c r="E50" s="5">
-        <v>0.52674799999999999</v>
+        <v>26.469477999999999</v>
       </c>
       <c r="F50" s="3">
-        <v>2777.407811</v>
+        <v>2803.30294</v>
       </c>
       <c r="G50" s="5">
-        <v>405.49374799999998</v>
+        <v>408.62409100000002</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -3835,7 +3873,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="3">
-        <v>9.9999999999999995E-7</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="E51" s="5">
         <v>0</v>
@@ -3854,16 +3892,16 @@
         <v>4</v>
       </c>
       <c r="D52" s="3">
-        <v>2841.3727509999999</v>
+        <v>2823.2492350000002</v>
       </c>
       <c r="E52" s="5">
-        <v>409.66006700000003</v>
+        <v>406.83753200000001</v>
       </c>
       <c r="F52" s="3">
-        <v>3033.5100109999998</v>
+        <v>3036.0300050000001</v>
       </c>
       <c r="G52" s="5">
-        <v>439.16754700000001</v>
+        <v>439.83434199999999</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -3875,7 +3913,7 @@
         <v>5</v>
       </c>
       <c r="D53" s="3">
-        <v>1.9999999999999999E-6</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E53" s="5">
         <v>0</v>
@@ -3894,16 +3932,16 @@
         <v>4</v>
       </c>
       <c r="D54" s="3">
-        <v>2702.361081</v>
+        <v>2696.1022630000002</v>
       </c>
       <c r="E54" s="5">
-        <v>391.2876</v>
+        <v>389.06899099999998</v>
       </c>
       <c r="F54" s="3">
-        <v>2911.3941690000001</v>
+        <v>2901.2581759999998</v>
       </c>
       <c r="G54" s="5">
-        <v>420.69542999999999</v>
+        <v>420.20660400000003</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -3934,16 +3972,16 @@
         <v>4</v>
       </c>
       <c r="D56" s="3">
-        <v>2803.6823370000002</v>
+        <v>2799.358577</v>
       </c>
       <c r="E56" s="5">
-        <v>405.61871300000001</v>
+        <v>403.90938699999998</v>
       </c>
       <c r="F56" s="3">
-        <v>3001.708537</v>
+        <v>3002.136904</v>
       </c>
       <c r="G56" s="5">
-        <v>435.38002299999999</v>
+        <v>434.75509199999999</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -3974,16 +4012,16 @@
         <v>4</v>
       </c>
       <c r="D58" s="3">
-        <v>6.6198899999999998</v>
+        <v>123.736752</v>
       </c>
       <c r="E58" s="5">
-        <v>0.52680000000000005</v>
+        <v>26.468942999999999</v>
       </c>
       <c r="F58" s="3">
-        <v>2776.7977230000001</v>
+        <v>2802.6805410000002</v>
       </c>
       <c r="G58" s="5">
-        <v>405.492501</v>
+        <v>408.62439799999999</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -3997,16 +4035,16 @@
         <v>5</v>
       </c>
       <c r="D59" s="3">
-        <v>2.31E-4</v>
+        <v>4.6299999999999998E-4</v>
       </c>
       <c r="E59" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="F59" s="3">
-        <v>7.2999999999999999E-5</v>
+        <v>6.3E-5</v>
       </c>
       <c r="G59" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -4016,16 +4054,16 @@
         <v>4</v>
       </c>
       <c r="D60" s="3">
-        <v>5.3887999999999998E-2</v>
+        <v>5.3657000000000003E-2</v>
       </c>
       <c r="E60" s="5">
-        <v>2.4000000000000001E-5</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="F60" s="3">
-        <v>5.2610999999999998E-2</v>
+        <v>5.2618999999999999E-2</v>
       </c>
       <c r="G60" s="5">
-        <v>3.6999999999999998E-5</v>
+        <v>5.5000000000000002E-5</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -4037,16 +4075,16 @@
         <v>5</v>
       </c>
       <c r="D61" s="3">
-        <v>9.8999999999999994E-5</v>
+        <v>2.31E-4</v>
       </c>
       <c r="E61" s="5">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="F61" s="3">
+        <v>5.3999999999999998E-5</v>
+      </c>
+      <c r="G61" s="5">
         <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="F61" s="3">
-        <v>4.8999999999999998E-5</v>
-      </c>
-      <c r="G61" s="5">
-        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -4056,16 +4094,16 @@
         <v>4</v>
       </c>
       <c r="D62" s="3">
-        <v>7.7285999999999994E-2</v>
+        <v>7.7171000000000003E-2</v>
       </c>
       <c r="E62" s="5">
-        <v>4.5000000000000003E-5</v>
+        <v>4.6999999999999997E-5</v>
       </c>
       <c r="F62" s="3">
-        <v>7.6022000000000006E-2</v>
+        <v>7.5729000000000005E-2</v>
       </c>
       <c r="G62" s="5">
-        <v>9.5000000000000005E-5</v>
+        <v>1.08E-4</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -4077,16 +4115,16 @@
         <v>5</v>
       </c>
       <c r="D63" s="3">
-        <v>1.7699999999999999E-4</v>
+        <v>3.3799999999999998E-4</v>
       </c>
       <c r="E63" s="5">
-        <v>7.9999999999999996E-6</v>
+        <v>2.0999999999999999E-5</v>
       </c>
       <c r="F63" s="3">
-        <v>6.7999999999999999E-5</v>
+        <v>6.4999999999999994E-5</v>
       </c>
       <c r="G63" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>3.0000000000000001E-6</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -4096,16 +4134,16 @@
         <v>4</v>
       </c>
       <c r="D64" s="3">
-        <v>0.174374</v>
+        <v>0.174567</v>
       </c>
       <c r="E64" s="5">
-        <v>4.75E-4</v>
+        <v>3.2000000000000003E-4</v>
       </c>
       <c r="F64" s="3">
-        <v>0.17039299999999999</v>
+        <v>0.17083699999999999</v>
       </c>
       <c r="G64" s="5">
-        <v>3.6699999999999998E-4</v>
+        <v>2.8400000000000002E-4</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -4117,16 +4155,16 @@
         <v>5</v>
       </c>
       <c r="D65" s="3">
-        <v>1.08E-4</v>
+        <v>2.63E-4</v>
       </c>
       <c r="E65" s="5">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="G65" s="5">
         <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="F65" s="3">
-        <v>8.2000000000000001E-5</v>
-      </c>
-      <c r="G65" s="5">
-        <v>3.9999999999999998E-6</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -4136,16 +4174,16 @@
         <v>4</v>
       </c>
       <c r="D66" s="3">
-        <v>0.40284399999999998</v>
+        <v>0.42796000000000001</v>
       </c>
       <c r="E66" s="5">
-        <v>3.8499999999999998E-4</v>
+        <v>8.7600000000000004E-4</v>
       </c>
       <c r="F66" s="3">
-        <v>0.61008799999999996</v>
+        <v>0.62239900000000004</v>
       </c>
       <c r="G66" s="5">
-        <v>2.1909999999999998E-3</v>
+        <v>1.66E-3</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -4159,16 +4197,16 @@
         <v>5</v>
       </c>
       <c r="D67" s="3">
-        <v>4.3020000000000003E-3</v>
+        <v>8.7180000000000001E-3</v>
       </c>
       <c r="E67" s="5">
-        <v>4.3999999999999999E-5</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="F67" s="3">
-        <v>1.397E-3</v>
+        <v>1.191E-3</v>
       </c>
       <c r="G67" s="5">
-        <v>3.0000000000000001E-5</v>
+        <v>2.5999999999999998E-5</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -4178,16 +4216,16 @@
         <v>4</v>
       </c>
       <c r="D68" s="3">
-        <v>52748.503445000002</v>
+        <v>52618.328254</v>
       </c>
       <c r="E68" s="5">
-        <v>7615.7066590000004</v>
+        <v>7592.2179109999997</v>
       </c>
       <c r="F68" s="3">
-        <v>57611.793489000003</v>
+        <v>57630.283911999999</v>
       </c>
       <c r="G68" s="5">
-        <v>8337.461464</v>
+        <v>8346.369788</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -4199,16 +4237,16 @@
         <v>5</v>
       </c>
       <c r="D69" s="3">
-        <v>1.302E-3</v>
+        <v>3.0070000000000001E-3</v>
       </c>
       <c r="E69" s="5">
-        <v>3.0000000000000001E-5</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="F69" s="3">
-        <v>6.5099999999999999E-4</v>
+        <v>7.1199999999999996E-4</v>
       </c>
       <c r="G69" s="5">
-        <v>6.9999999999999999E-6</v>
+        <v>2.3E-5</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -4218,16 +4256,16 @@
         <v>4</v>
       </c>
       <c r="D70" s="3">
-        <v>34953.479749999999</v>
+        <v>34950.766192000003</v>
       </c>
       <c r="E70" s="5">
-        <v>5056.1667660000003</v>
+        <v>5044.5809360000003</v>
       </c>
       <c r="F70" s="3">
-        <v>38375.066978000003</v>
+        <v>38340.915735000002</v>
       </c>
       <c r="G70" s="5">
-        <v>5555.1075510000001</v>
+        <v>5551.9700590000002</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -4239,16 +4277,16 @@
         <v>5</v>
       </c>
       <c r="D71" s="3">
-        <v>1.0139999999999999E-3</v>
+        <v>1.9350000000000001E-3</v>
       </c>
       <c r="E71" s="5">
-        <v>4.6E-5</v>
+        <v>1.21E-4</v>
       </c>
       <c r="F71" s="3">
-        <v>3.9899999999999999E-4</v>
+        <v>3.8200000000000002E-4</v>
       </c>
       <c r="G71" s="5">
-        <v>1.4E-5</v>
+        <v>1.9000000000000001E-5</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -4258,16 +4296,16 @@
         <v>4</v>
       </c>
       <c r="D72" s="3">
-        <v>16003.439263</v>
+        <v>15984.410964000001</v>
       </c>
       <c r="E72" s="5">
-        <v>2296.6714830000001</v>
+        <v>2292.0878459999999</v>
       </c>
       <c r="F72" s="3">
-        <v>17539.091582000001</v>
+        <v>17537.59388</v>
       </c>
       <c r="G72" s="5">
-        <v>2525.5785609999998</v>
+        <v>2526.3970629999999</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -4279,16 +4317,16 @@
         <v>5</v>
       </c>
       <c r="D73" s="3">
-        <v>2.5900000000000001E-4</v>
+        <v>6.1300000000000005E-4</v>
       </c>
       <c r="E73" s="5">
-        <v>1.2E-5</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="F73" s="3">
-        <v>1.34E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="G73" s="5">
-        <v>6.9999999999999999E-6</v>
+        <v>9.0000000000000002E-6</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -4298,16 +4336,16 @@
         <v>4</v>
       </c>
       <c r="D74" s="3">
-        <v>16.822747</v>
+        <v>288.787553</v>
       </c>
       <c r="E74" s="5">
-        <v>1.285174</v>
+        <v>61.354892999999997</v>
       </c>
       <c r="F74" s="3">
-        <v>4530.884814</v>
+        <v>4508.3483759999999</v>
       </c>
       <c r="G74" s="5">
-        <v>660.33826399999998</v>
+        <v>661.37694599999998</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -4321,16 +4359,16 @@
         <v>5</v>
       </c>
       <c r="D75" s="3">
-        <v>2.0000000000000002E-5</v>
+        <v>9.1000000000000003E-5</v>
       </c>
       <c r="E75" s="5">
-        <v>3.0000000000000001E-6</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="F75" s="3">
-        <v>3.0000000000000001E-6</v>
+        <v>0</v>
       </c>
       <c r="G75" s="5">
-        <v>9.9999999999999995E-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -4340,16 +4378,16 @@
         <v>4</v>
       </c>
       <c r="D76" s="3">
-        <v>52747.503500999999</v>
+        <v>52617.328292999999</v>
       </c>
       <c r="E76" s="5">
-        <v>7615.7066439999999</v>
+        <v>7592.217901</v>
       </c>
       <c r="F76" s="3">
-        <v>57610.793550000002</v>
+        <v>57629.283971999997</v>
       </c>
       <c r="G76" s="5">
-        <v>8337.461448</v>
+        <v>8346.369772</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -4361,10 +4399,10 @@
         <v>5</v>
       </c>
       <c r="D77" s="3">
-        <v>2.0999999999999999E-5</v>
+        <v>1.2999999999999999E-5</v>
       </c>
       <c r="E77" s="5">
-        <v>3.9999999999999998E-6</v>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="F77" s="3">
         <v>0</v>
@@ -4380,16 +4418,16 @@
         <v>4</v>
       </c>
       <c r="D78" s="3">
-        <v>34952.479776</v>
+        <v>34949.766215000003</v>
       </c>
       <c r="E78" s="5">
-        <v>5056.1667589999997</v>
+        <v>5044.5809300000001</v>
       </c>
       <c r="F78" s="3">
-        <v>38374.067015000001</v>
+        <v>38339.915772</v>
       </c>
       <c r="G78" s="5">
-        <v>5555.1075410000003</v>
+        <v>5551.9700499999999</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -4420,16 +4458,16 @@
         <v>4</v>
       </c>
       <c r="D80" s="3">
-        <v>16002.439387</v>
+        <v>15983.411050999999</v>
       </c>
       <c r="E80" s="5">
-        <v>2296.6714499999998</v>
+        <v>2292.0878229999998</v>
       </c>
       <c r="F80" s="3">
-        <v>17538.091767000002</v>
+        <v>17536.594067999999</v>
       </c>
       <c r="G80" s="5">
-        <v>2525.5785129999999</v>
+        <v>2526.3970129999998</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -4460,16 +4498,16 @@
         <v>4</v>
       </c>
       <c r="D82" s="3">
-        <v>15.860037</v>
+        <v>287.78862099999998</v>
       </c>
       <c r="E82" s="5">
-        <v>1.283331</v>
+        <v>61.354733000000003</v>
       </c>
       <c r="F82" s="3">
-        <v>4529.885233</v>
+        <v>4507.3488589999997</v>
       </c>
       <c r="G82" s="5">
-        <v>660.33815500000003</v>
+        <v>661.37682099999995</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -4483,13 +4521,13 @@
         <v>5</v>
       </c>
       <c r="D83" s="3">
-        <v>2.0929999999999998E-3</v>
+        <v>2.9710000000000001E-3</v>
       </c>
       <c r="E83" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>2.9E-5</v>
       </c>
       <c r="F83" s="3">
-        <v>1.194E-3</v>
+        <v>1.1039999999999999E-3</v>
       </c>
       <c r="G83" s="5">
         <v>9.9999999999999995E-7</v>
@@ -4505,7 +4543,7 @@
         <v>3.1983999999999999E-2</v>
       </c>
       <c r="E84" s="5">
-        <v>9.9999999999999995E-7</v>
+        <v>0</v>
       </c>
       <c r="F84" s="3">
         <v>3.1983999999999999E-2</v>
@@ -4523,16 +4561,16 @@
         <v>5</v>
       </c>
       <c r="D85" s="3">
-        <v>1.145E-3</v>
+        <v>1.75E-3</v>
       </c>
       <c r="E85" s="5">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="F85" s="3">
+        <v>8.5300000000000003E-4</v>
+      </c>
+      <c r="G85" s="5">
         <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="F85" s="3">
-        <v>8.1599999999999999E-4</v>
-      </c>
-      <c r="G85" s="5">
-        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -4563,13 +4601,13 @@
         <v>5</v>
       </c>
       <c r="D87" s="3">
-        <v>1.018E-3</v>
+        <v>1.407E-3</v>
       </c>
       <c r="E87" s="5">
-        <v>1.9999999999999999E-6</v>
+        <v>1.4E-5</v>
       </c>
       <c r="F87" s="3">
-        <v>6.3900000000000003E-4</v>
+        <v>6.2500000000000001E-4</v>
       </c>
       <c r="G87" s="5">
         <v>0</v>
@@ -4585,7 +4623,7 @@
         <v>3.1982999999999998E-2</v>
       </c>
       <c r="E88" s="5">
-        <v>3.0000000000000001E-6</v>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="F88" s="3">
         <v>3.1981999999999997E-2</v>
@@ -4603,13 +4641,13 @@
         <v>5</v>
       </c>
       <c r="D89" s="3">
-        <v>5.1400000000000003E-4</v>
+        <v>7.9199999999999995E-4</v>
       </c>
       <c r="E89" s="5">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F89" s="3">
-        <v>3.7100000000000002E-4</v>
+        <v>4.0400000000000001E-4</v>
       </c>
       <c r="G89" s="5">
         <v>0</v>
@@ -4622,469 +4660,469 @@
         <v>4</v>
       </c>
       <c r="D90" s="2">
-        <v>3.1383000000000001E-2</v>
+        <v>3.1967000000000002E-2</v>
       </c>
       <c r="E90" s="4">
-        <v>4.3049999999999998E-3</v>
+        <v>9.2999999999999997E-5</v>
       </c>
       <c r="F90" s="2">
-        <v>3.1977999999999999E-2</v>
+        <v>3.1976999999999998E-2</v>
       </c>
       <c r="G90" s="4">
-        <v>4.0000000000000003E-5</v>
+        <v>5.3000000000000001E-5</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="19"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
-      <c r="E91" s="19"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="21"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="25"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="25" t="s">
+      <c r="A92" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="29" t="s">
+      <c r="C92" s="17"/>
+      <c r="D92" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E92" s="30"/>
-      <c r="F92" s="29" t="s">
+      <c r="E92" s="29"/>
+      <c r="F92" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G92" s="30"/>
+      <c r="G92" s="29"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C93" s="16"/>
-      <c r="D93" s="7">
+      <c r="C93" s="35"/>
+      <c r="D93" s="33">
         <v>4060.3968249999998</v>
       </c>
-      <c r="E93" s="6">
-        <v>14.253318</v>
-      </c>
-      <c r="F93" s="7">
+      <c r="E93" s="36">
+        <v>14.273114</v>
+      </c>
+      <c r="F93" s="33">
         <v>4060.3968249999998</v>
       </c>
-      <c r="G93" s="6">
+      <c r="G93" s="36">
         <v>14.233064000000001</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="3"/>
-      <c r="B94" s="10" t="s">
+      <c r="A94" s="37"/>
+      <c r="B94" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="3">
+      <c r="C94" s="39"/>
+      <c r="D94" s="37">
         <v>3166.8412699999999</v>
       </c>
-      <c r="E94" s="5">
-        <v>14.355065</v>
-      </c>
-      <c r="F94" s="3">
+      <c r="E94" s="40">
+        <v>14.345655000000001</v>
+      </c>
+      <c r="F94" s="37">
         <v>3166.8412699999999</v>
       </c>
-      <c r="G94" s="5">
+      <c r="G94" s="40">
         <v>14.342587999999999</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="3"/>
-      <c r="B95" s="10" t="s">
+      <c r="A95" s="37"/>
+      <c r="B95" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="3">
+      <c r="C95" s="39"/>
+      <c r="D95" s="37">
         <v>1013.555556</v>
       </c>
-      <c r="E95" s="5">
+      <c r="E95" s="40">
         <v>8.5249260000000007</v>
       </c>
-      <c r="F95" s="3">
+      <c r="F95" s="37">
         <v>1013.555556</v>
       </c>
-      <c r="G95" s="5">
+      <c r="G95" s="40">
         <v>8.5215650000000007</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="3"/>
-      <c r="B96" s="10" t="s">
+      <c r="A96" s="37"/>
+      <c r="B96" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="3">
+      <c r="C96" s="39"/>
+      <c r="D96" s="37">
         <v>289.79365100000001</v>
       </c>
-      <c r="E96" s="5">
+      <c r="E96" s="40">
+        <v>4.1700710000000001</v>
+      </c>
+      <c r="F96" s="37">
+        <v>289.79365100000001</v>
+      </c>
+      <c r="G96" s="40">
         <v>4.1681080000000001</v>
       </c>
-      <c r="F96" s="3">
-        <v>289.79365100000001</v>
-      </c>
-      <c r="G96" s="5">
-        <v>4.1681080000000001</v>
-      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B97" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="11"/>
-      <c r="D97" s="3">
+      <c r="C97" s="39"/>
+      <c r="D97" s="37">
+        <v>3736.2698409999998</v>
+      </c>
+      <c r="E97" s="40">
+        <v>15.112171999999999</v>
+      </c>
+      <c r="F97" s="37">
         <v>3736.3492059999999</v>
       </c>
-      <c r="E97" s="5">
-        <v>15.062398999999999</v>
-      </c>
-      <c r="F97" s="3">
-        <v>3736.3492059999999</v>
-      </c>
-      <c r="G97" s="5">
+      <c r="G97" s="40">
         <v>15.009328999999999</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="3"/>
-      <c r="B98" s="10" t="s">
+      <c r="A98" s="37"/>
+      <c r="B98" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="3">
-        <v>1625.142857</v>
-      </c>
-      <c r="E98" s="5">
-        <v>10.135713000000001</v>
-      </c>
-      <c r="F98" s="3">
+      <c r="C98" s="39"/>
+      <c r="D98" s="37">
         <v>1625.1746029999999</v>
       </c>
-      <c r="G98" s="5">
+      <c r="E98" s="40">
+        <v>10.130330000000001</v>
+      </c>
+      <c r="F98" s="37">
+        <v>1625.1746029999999</v>
+      </c>
+      <c r="G98" s="40">
         <v>10.212201</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="3"/>
-      <c r="B99" s="10" t="s">
+      <c r="A99" s="37"/>
+      <c r="B99" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="11"/>
-      <c r="D99" s="3">
+      <c r="C99" s="39"/>
+      <c r="D99" s="37">
         <v>490.25396799999999</v>
       </c>
-      <c r="E99" s="5">
+      <c r="E99" s="40">
         <v>5.261431</v>
       </c>
-      <c r="F99" s="3">
+      <c r="F99" s="37">
         <v>490.23809499999999</v>
       </c>
-      <c r="G99" s="5">
+      <c r="G99" s="40">
         <v>5.2168609999999997</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="3"/>
-      <c r="B100" s="10" t="s">
+      <c r="A100" s="37"/>
+      <c r="B100" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C100" s="11"/>
-      <c r="D100" s="3">
-        <v>74.666667000000004</v>
-      </c>
-      <c r="E100" s="5">
-        <v>2.1451129999999998</v>
-      </c>
-      <c r="F100" s="3">
+      <c r="C100" s="39"/>
+      <c r="D100" s="37">
+        <v>74.714286000000001</v>
+      </c>
+      <c r="E100" s="40">
+        <v>2.0154990000000002</v>
+      </c>
+      <c r="F100" s="37">
         <v>74.571428999999995</v>
       </c>
-      <c r="G100" s="5">
+      <c r="G100" s="40">
         <v>1.824362</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="39"/>
+      <c r="D101" s="37">
+        <v>0</v>
+      </c>
+      <c r="E101" s="40">
+        <v>0</v>
+      </c>
+      <c r="F101" s="37">
+        <v>0</v>
+      </c>
+      <c r="G101" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" s="37"/>
+      <c r="B102" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="39"/>
+      <c r="D102" s="37">
+        <v>1.5873000000000002E-2</v>
+      </c>
+      <c r="E102" s="40">
+        <v>3.1730000000000001E-2</v>
+      </c>
+      <c r="F102" s="37">
+        <v>0</v>
+      </c>
+      <c r="G102" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="37"/>
+      <c r="B103" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="39"/>
+      <c r="D103" s="37">
+        <v>1.5873000000000002E-2</v>
+      </c>
+      <c r="E103" s="40">
+        <v>3.1730000000000001E-2</v>
+      </c>
+      <c r="F103" s="37">
+        <v>0</v>
+      </c>
+      <c r="G103" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="37"/>
+      <c r="B104" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" s="39"/>
+      <c r="D104" s="37">
+        <v>0.61904800000000004</v>
+      </c>
+      <c r="E104" s="40">
+        <v>0.45103599999999999</v>
+      </c>
+      <c r="F104" s="37">
+        <v>0</v>
+      </c>
+      <c r="G104" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B101" s="10" t="s">
+      <c r="B105" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C101" s="11"/>
-      <c r="D101" s="3">
-        <v>0</v>
-      </c>
-      <c r="E101" s="5">
-        <v>0</v>
-      </c>
-      <c r="F101" s="3">
-        <v>0</v>
-      </c>
-      <c r="G101" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="3"/>
-      <c r="B102" s="10" t="s">
+      <c r="C105" s="39"/>
+      <c r="D105" s="37">
+        <v>9.0015999999999999E-2</v>
+      </c>
+      <c r="E105" s="40">
+        <v>4.8999999999999998E-5</v>
+      </c>
+      <c r="F105" s="37">
+        <v>9.0015999999999999E-2</v>
+      </c>
+      <c r="G105" s="40">
+        <v>4.8999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="37"/>
+      <c r="B106" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C102" s="11"/>
-      <c r="D102" s="3">
-        <v>0</v>
-      </c>
-      <c r="E102" s="5">
-        <v>0</v>
-      </c>
-      <c r="F102" s="3">
-        <v>0</v>
-      </c>
-      <c r="G102" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="3"/>
-      <c r="B103" s="10" t="s">
+      <c r="C106" s="39"/>
+      <c r="D106" s="37">
+        <v>0.114798</v>
+      </c>
+      <c r="E106" s="40">
+        <v>8.7000000000000001E-5</v>
+      </c>
+      <c r="F106" s="37">
+        <v>0.114799</v>
+      </c>
+      <c r="G106" s="40">
+        <v>8.7000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" s="37"/>
+      <c r="B107" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="11"/>
-      <c r="D103" s="3">
-        <v>1.5873000000000002E-2</v>
-      </c>
-      <c r="E103" s="5">
-        <v>3.1730000000000001E-2</v>
-      </c>
-      <c r="F103" s="3">
-        <v>0</v>
-      </c>
-      <c r="G103" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="3"/>
-      <c r="B104" s="10" t="s">
+      <c r="C107" s="39"/>
+      <c r="D107" s="37">
+        <v>0.36002899999999999</v>
+      </c>
+      <c r="E107" s="40">
+        <v>3.2600000000000001E-4</v>
+      </c>
+      <c r="F107" s="37">
+        <v>0.36002699999999999</v>
+      </c>
+      <c r="G107" s="40">
+        <v>3.2600000000000001E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="37"/>
+      <c r="B108" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="3">
-        <v>7.9682539999999999</v>
-      </c>
-      <c r="E104" s="5">
-        <v>1.5708089999999999</v>
-      </c>
-      <c r="F104" s="3">
-        <v>0</v>
-      </c>
-      <c r="G104" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B105" s="10" t="s">
+      <c r="C108" s="39"/>
+      <c r="D108" s="37">
+        <v>1.2583150000000001</v>
+      </c>
+      <c r="E108" s="40">
+        <v>2.5439999999999998E-3</v>
+      </c>
+      <c r="F108" s="37">
+        <v>1.2583150000000001</v>
+      </c>
+      <c r="G108" s="40">
+        <v>2.5430000000000001E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="11"/>
-      <c r="D105" s="3">
-        <v>9.0015999999999999E-2</v>
-      </c>
-      <c r="E105" s="5">
-        <v>4.8999999999999998E-5</v>
-      </c>
-      <c r="F105" s="3">
-        <v>9.0015999999999999E-2</v>
-      </c>
-      <c r="G105" s="5">
-        <v>4.8999999999999998E-5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="3"/>
-      <c r="B106" s="10" t="s">
+      <c r="C109" s="39"/>
+      <c r="D109" s="37">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="E109" s="40">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="F109" s="37">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G109" s="40">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="37"/>
+      <c r="B110" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="3">
-        <v>0.114798</v>
-      </c>
-      <c r="E106" s="5">
-        <v>8.7000000000000001E-5</v>
-      </c>
-      <c r="F106" s="3">
-        <v>0.114799</v>
-      </c>
-      <c r="G106" s="5">
-        <v>8.7000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="3"/>
-      <c r="B107" s="10" t="s">
+      <c r="C110" s="39"/>
+      <c r="D110" s="37">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="E110" s="40">
+        <v>1.7E-5</v>
+      </c>
+      <c r="F110" s="37">
+        <v>0</v>
+      </c>
+      <c r="G110" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="37"/>
+      <c r="B111" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C107" s="11"/>
-      <c r="D107" s="3">
-        <v>0.36002800000000001</v>
-      </c>
-      <c r="E107" s="5">
-        <v>3.2499999999999999E-4</v>
-      </c>
-      <c r="F107" s="3">
-        <v>0.36002699999999999</v>
-      </c>
-      <c r="G107" s="5">
-        <v>3.2600000000000001E-4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="3"/>
-      <c r="B108" s="10" t="s">
+      <c r="C111" s="39"/>
+      <c r="D111" s="37">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="E111" s="40">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F111" s="37">
+        <v>0</v>
+      </c>
+      <c r="G111" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="41"/>
+      <c r="B112" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C108" s="11"/>
-      <c r="D108" s="3">
-        <v>1.258318</v>
-      </c>
-      <c r="E108" s="5">
-        <v>2.542E-3</v>
-      </c>
-      <c r="F108" s="3">
-        <v>1.2583150000000001</v>
-      </c>
-      <c r="G108" s="5">
-        <v>2.5430000000000001E-3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C109" s="11"/>
-      <c r="D109" s="3">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="E109" s="5">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="F109" s="3">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G109" s="5">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="3"/>
-      <c r="B110" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="11"/>
-      <c r="D110" s="3">
-        <v>0</v>
-      </c>
-      <c r="E110" s="5">
-        <v>0</v>
-      </c>
-      <c r="F110" s="3">
-        <v>0</v>
-      </c>
-      <c r="G110" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="3"/>
-      <c r="B111" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C111" s="11"/>
-      <c r="D111" s="3">
-        <v>0</v>
-      </c>
-      <c r="E111" s="5">
-        <v>0</v>
-      </c>
-      <c r="F111" s="3">
-        <v>0</v>
-      </c>
-      <c r="G111" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="2"/>
-      <c r="B112" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C112" s="13"/>
-      <c r="D112" s="2">
-        <v>8.2439999999999996E-3</v>
-      </c>
-      <c r="E112" s="4">
-        <v>6.4099999999999997E-4</v>
-      </c>
-      <c r="F112" s="2">
-        <v>0</v>
-      </c>
-      <c r="G112" s="4">
+      <c r="C112" s="43"/>
+      <c r="D112" s="41">
+        <v>2.99E-4</v>
+      </c>
+      <c r="E112" s="44">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="F112" s="41">
+        <v>0</v>
+      </c>
+      <c r="G112" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B113" s="19"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="21"/>
+      <c r="B113" s="24"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="25"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="25" t="s">
+      <c r="A114" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B114" s="25" t="s">
+      <c r="B114" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C114" s="26" t="s">
+      <c r="C114" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D114" s="27" t="s">
+      <c r="D114" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E114" s="28"/>
-      <c r="F114" s="29" t="s">
+      <c r="E114" s="27"/>
+      <c r="F114" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G114" s="30"/>
+      <c r="G114" s="29"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>9</v>
@@ -5092,10 +5130,18 @@
       <c r="C115" t="s">
         <v>5</v>
       </c>
-      <c r="D115" s="7"/>
-      <c r="E115" s="6"/>
-      <c r="F115" s="7"/>
-      <c r="G115" s="6"/>
+      <c r="D115" s="7">
+        <v>16.539683</v>
+      </c>
+      <c r="E115" s="6">
+        <v>1.138781</v>
+      </c>
+      <c r="F115" s="7">
+        <v>17.761904999999999</v>
+      </c>
+      <c r="G115" s="6">
+        <v>1.3851309999999999</v>
+      </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
@@ -5103,10 +5149,18 @@
       <c r="C116" t="s">
         <v>4</v>
       </c>
-      <c r="D116" s="3"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="3"/>
-      <c r="G116" s="5"/>
+      <c r="D116" s="3">
+        <v>6789.4761900000003</v>
+      </c>
+      <c r="E116" s="5">
+        <v>21.879121000000001</v>
+      </c>
+      <c r="F116" s="3">
+        <v>6909.3968249999998</v>
+      </c>
+      <c r="G116" s="5">
+        <v>27.063161000000001</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
@@ -5116,10 +5170,18 @@
       <c r="C117" t="s">
         <v>5</v>
       </c>
-      <c r="D117" s="3"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="5"/>
+      <c r="D117" s="3">
+        <v>9.6031750000000002</v>
+      </c>
+      <c r="E117" s="5">
+        <v>0.86244500000000002</v>
+      </c>
+      <c r="F117" s="3">
+        <v>9.7619050000000005</v>
+      </c>
+      <c r="G117" s="5">
+        <v>0.83247700000000002</v>
+      </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="3"/>
@@ -5127,10 +5189,18 @@
       <c r="C118" t="s">
         <v>4</v>
       </c>
-      <c r="D118" s="3"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="5"/>
+      <c r="D118" s="3">
+        <v>4720.6349209999998</v>
+      </c>
+      <c r="E118" s="5">
+        <v>21.549402000000001</v>
+      </c>
+      <c r="F118" s="3">
+        <v>4810.7301589999997</v>
+      </c>
+      <c r="G118" s="5">
+        <v>21.257791999999998</v>
+      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="3"/>
@@ -5140,10 +5210,18 @@
       <c r="C119" t="s">
         <v>5</v>
       </c>
-      <c r="D119" s="3"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="5"/>
+      <c r="D119" s="3">
+        <v>5.4444439999999998</v>
+      </c>
+      <c r="E119" s="5">
+        <v>0.64570499999999997</v>
+      </c>
+      <c r="F119" s="3">
+        <v>5.5873020000000002</v>
+      </c>
+      <c r="G119" s="5">
+        <v>0.62943000000000005</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
@@ -5151,10 +5229,18 @@
       <c r="C120" t="s">
         <v>4</v>
       </c>
-      <c r="D120" s="3"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="5"/>
+      <c r="D120" s="3">
+        <v>2067.3492059999999</v>
+      </c>
+      <c r="E120" s="5">
+        <v>17.082284000000001</v>
+      </c>
+      <c r="F120" s="3">
+        <v>2112.7777780000001</v>
+      </c>
+      <c r="G120" s="5">
+        <v>16.910822</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
@@ -5164,10 +5250,18 @@
       <c r="C121" t="s">
         <v>5</v>
       </c>
-      <c r="D121" s="3"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="5"/>
+      <c r="D121" s="3">
+        <v>1.730159</v>
+      </c>
+      <c r="E121" s="5">
+        <v>0.387017</v>
+      </c>
+      <c r="F121" s="3">
+        <v>1.9206350000000001</v>
+      </c>
+      <c r="G121" s="5">
+        <v>0.39511400000000002</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
@@ -5175,14 +5269,22 @@
       <c r="C122" t="s">
         <v>4</v>
       </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="33"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="5"/>
+      <c r="D122" s="3">
+        <v>844.79365099999995</v>
+      </c>
+      <c r="E122">
+        <v>9.4963639999999998</v>
+      </c>
+      <c r="F122" s="3">
+        <v>589</v>
+      </c>
+      <c r="G122" s="5">
+        <v>14.561306</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>9</v>
@@ -5190,10 +5292,18 @@
       <c r="C123" t="s">
         <v>5</v>
       </c>
-      <c r="D123" s="3"/>
-      <c r="E123" s="33"/>
-      <c r="F123" s="3"/>
-      <c r="G123" s="5"/>
+      <c r="D123" s="3">
+        <v>14.460317</v>
+      </c>
+      <c r="E123">
+        <v>0.97731100000000004</v>
+      </c>
+      <c r="F123" s="3">
+        <v>14.222222</v>
+      </c>
+      <c r="G123" s="5">
+        <v>1.057374</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
@@ -5201,10 +5311,18 @@
       <c r="C124" t="s">
         <v>4</v>
       </c>
-      <c r="D124" s="3"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="5"/>
+      <c r="D124" s="3">
+        <v>5902.2222220000003</v>
+      </c>
+      <c r="E124" s="5">
+        <v>21.785903000000001</v>
+      </c>
+      <c r="F124" s="3">
+        <v>5554.0158730000003</v>
+      </c>
+      <c r="G124" s="5">
+        <v>32.496398999999997</v>
+      </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="3"/>
@@ -5214,10 +5332,18 @@
       <c r="C125" t="s">
         <v>5</v>
       </c>
-      <c r="D125" s="3"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="3"/>
-      <c r="G125" s="5"/>
+      <c r="D125" s="3">
+        <v>8.0793649999999992</v>
+      </c>
+      <c r="E125" s="5">
+        <v>0.70988700000000005</v>
+      </c>
+      <c r="F125" s="3">
+        <v>7.7777779999999996</v>
+      </c>
+      <c r="G125" s="5">
+        <v>0.59742600000000001</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
@@ -5225,10 +5351,18 @@
       <c r="C126" t="s">
         <v>4</v>
       </c>
-      <c r="D126" s="3"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="5"/>
+      <c r="D126" s="3">
+        <v>4100.9206350000004</v>
+      </c>
+      <c r="E126" s="5">
+        <v>21.169836</v>
+      </c>
+      <c r="F126" s="3">
+        <v>3864.8412699999999</v>
+      </c>
+      <c r="G126" s="5">
+        <v>28.320315000000001</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
@@ -5238,10 +5372,18 @@
       <c r="C127" t="s">
         <v>5</v>
       </c>
-      <c r="D127" s="3"/>
-      <c r="E127" s="5"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="5"/>
+      <c r="D127" s="3">
+        <v>4.6190480000000003</v>
+      </c>
+      <c r="E127" s="5">
+        <v>0.47961599999999999</v>
+      </c>
+      <c r="F127" s="3">
+        <v>4.5238100000000001</v>
+      </c>
+      <c r="G127" s="5">
+        <v>0.48265400000000003</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
@@ -5249,10 +5391,18 @@
       <c r="C128" t="s">
         <v>4</v>
       </c>
-      <c r="D128" s="3"/>
-      <c r="E128" s="5"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="5"/>
+      <c r="D128" s="3">
+        <v>1797.619048</v>
+      </c>
+      <c r="E128" s="5">
+        <v>15.740595000000001</v>
+      </c>
+      <c r="F128" s="3">
+        <v>1694.936508</v>
+      </c>
+      <c r="G128" s="5">
+        <v>17.414877000000001</v>
+      </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
@@ -5262,10 +5412,18 @@
       <c r="C129" t="s">
         <v>5</v>
       </c>
-      <c r="D129" s="3"/>
-      <c r="E129" s="5"/>
-      <c r="F129" s="3"/>
-      <c r="G129" s="5"/>
+      <c r="D129" s="3">
+        <v>1.5396829999999999</v>
+      </c>
+      <c r="E129" s="5">
+        <v>0.334924</v>
+      </c>
+      <c r="F129" s="3">
+        <v>1.6507940000000001</v>
+      </c>
+      <c r="G129" s="5">
+        <v>0.29019299999999998</v>
+      </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
@@ -5273,14 +5431,22 @@
       <c r="C130" t="s">
         <v>4</v>
       </c>
-      <c r="D130" s="3"/>
-      <c r="E130" s="5"/>
-      <c r="F130" s="3"/>
-      <c r="G130" s="5"/>
+      <c r="D130" s="3">
+        <v>734.95238099999995</v>
+      </c>
+      <c r="E130" s="5">
+        <v>8.1207340000000006</v>
+      </c>
+      <c r="F130" s="3">
+        <v>474.15872999999999</v>
+      </c>
+      <c r="G130" s="5">
+        <v>10.807491000000001</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>9</v>
@@ -5288,10 +5454,18 @@
       <c r="C131" t="s">
         <v>5</v>
       </c>
-      <c r="D131" s="3"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="3"/>
-      <c r="G131" s="5"/>
+      <c r="D131" s="3">
+        <v>2.0793650000000001</v>
+      </c>
+      <c r="E131" s="5">
+        <v>0.47720600000000002</v>
+      </c>
+      <c r="F131" s="3">
+        <v>3.5396830000000001</v>
+      </c>
+      <c r="G131" s="5">
+        <v>0.54246700000000003</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
@@ -5299,10 +5473,18 @@
       <c r="C132" t="s">
         <v>4</v>
       </c>
-      <c r="D132" s="3"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="3"/>
-      <c r="G132" s="5"/>
+      <c r="D132" s="3">
+        <v>882.12698399999999</v>
+      </c>
+      <c r="E132" s="5">
+        <v>7.7088109999999999</v>
+      </c>
+      <c r="F132" s="3">
+        <v>1339.8888890000001</v>
+      </c>
+      <c r="G132" s="5">
+        <v>9.4755450000000003</v>
+      </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
@@ -5312,10 +5494,18 @@
       <c r="C133" t="s">
         <v>5</v>
       </c>
-      <c r="D133" s="3"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="3"/>
-      <c r="G133" s="5"/>
+      <c r="D133" s="3">
+        <v>1.5079370000000001</v>
+      </c>
+      <c r="E133" s="5">
+        <v>0.32578099999999999</v>
+      </c>
+      <c r="F133" s="3">
+        <v>1.9523809999999999</v>
+      </c>
+      <c r="G133" s="5">
+        <v>0.36587999999999998</v>
+      </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
@@ -5323,10 +5513,18 @@
       <c r="C134" t="s">
         <v>4</v>
       </c>
-      <c r="D134" s="3"/>
-      <c r="E134" s="5"/>
-      <c r="F134" s="3"/>
-      <c r="G134" s="5"/>
+      <c r="D134" s="3">
+        <v>616.031746</v>
+      </c>
+      <c r="E134" s="5">
+        <v>7.0179660000000004</v>
+      </c>
+      <c r="F134" s="3">
+        <v>935.26984100000004</v>
+      </c>
+      <c r="G134" s="5">
+        <v>9.7993120000000005</v>
+      </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
@@ -5336,10 +5534,18 @@
       <c r="C135" t="s">
         <v>5</v>
       </c>
-      <c r="D135" s="3"/>
-      <c r="E135" s="5"/>
-      <c r="F135" s="3"/>
-      <c r="G135" s="5"/>
+      <c r="D135" s="3">
+        <v>0.80952400000000002</v>
+      </c>
+      <c r="E135" s="5">
+        <v>0.24716099999999999</v>
+      </c>
+      <c r="F135" s="3">
+        <v>1.0634920000000001</v>
+      </c>
+      <c r="G135" s="5">
+        <v>0.312969</v>
+      </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
@@ -5347,10 +5553,18 @@
       <c r="C136" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="3"/>
-      <c r="E136" s="5"/>
-      <c r="F136" s="3"/>
-      <c r="G136" s="5"/>
+      <c r="D136" s="3">
+        <v>268.23809499999999</v>
+      </c>
+      <c r="E136" s="5">
+        <v>4.1985669999999997</v>
+      </c>
+      <c r="F136" s="3">
+        <v>413.23809499999999</v>
+      </c>
+      <c r="G136" s="5">
+        <v>6.0887919999999998</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
@@ -5360,10 +5574,18 @@
       <c r="C137" t="s">
         <v>5</v>
       </c>
-      <c r="D137" s="3"/>
-      <c r="E137" s="5"/>
-      <c r="F137" s="3"/>
-      <c r="G137" s="5"/>
+      <c r="D137" s="3">
+        <v>0.19047600000000001</v>
+      </c>
+      <c r="E137" s="5">
+        <v>0.118448</v>
+      </c>
+      <c r="F137" s="3">
+        <v>0.269841</v>
+      </c>
+      <c r="G137" s="5">
+        <v>0.151422</v>
+      </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
@@ -5371,10 +5593,18 @@
       <c r="C138" t="s">
         <v>4</v>
       </c>
-      <c r="D138" s="3"/>
-      <c r="E138" s="5"/>
-      <c r="F138" s="3"/>
-      <c r="G138" s="5"/>
+      <c r="D138" s="3">
+        <v>109.269841</v>
+      </c>
+      <c r="E138" s="5">
+        <v>3.3073359999999998</v>
+      </c>
+      <c r="F138" s="3">
+        <v>113.825397</v>
+      </c>
+      <c r="G138" s="5">
+        <v>4.1907199999999998</v>
+      </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
@@ -5386,9 +5616,13 @@
       <c r="C139" t="s">
         <v>5</v>
       </c>
-      <c r="D139" s="3"/>
+      <c r="D139" s="3">
+        <v>12.582781000000001</v>
+      </c>
       <c r="E139" s="5"/>
-      <c r="F139" s="3"/>
+      <c r="F139" s="3">
+        <v>19.699646999999999</v>
+      </c>
       <c r="G139" s="5"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -5397,9 +5631,13 @@
       <c r="C140" t="s">
         <v>4</v>
       </c>
-      <c r="D140" s="3"/>
+      <c r="D140" s="3">
+        <v>13.009186</v>
+      </c>
       <c r="E140" s="5"/>
-      <c r="F140" s="3"/>
+      <c r="F140" s="3">
+        <v>19.445817000000002</v>
+      </c>
       <c r="G140" s="5"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
@@ -5410,9 +5648,13 @@
       <c r="C141" t="s">
         <v>5</v>
       </c>
-      <c r="D141" s="3"/>
+      <c r="D141" s="3">
+        <v>15.625</v>
+      </c>
       <c r="E141" s="5"/>
-      <c r="F141" s="3"/>
+      <c r="F141" s="3">
+        <v>20.255182999999999</v>
+      </c>
       <c r="G141" s="5"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
@@ -5421,9 +5663,13 @@
       <c r="C142" t="s">
         <v>4</v>
       </c>
-      <c r="D142" s="3"/>
+      <c r="D142" s="3">
+        <v>13.057131</v>
+      </c>
       <c r="E142" s="5"/>
-      <c r="F142" s="3"/>
+      <c r="F142" s="3">
+        <v>19.478238000000001</v>
+      </c>
       <c r="G142" s="5"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
@@ -5434,9 +5680,13 @@
       <c r="C143" t="s">
         <v>5</v>
       </c>
-      <c r="D143" s="3"/>
+      <c r="D143" s="3">
+        <v>14.782609000000001</v>
+      </c>
       <c r="E143" s="5"/>
-      <c r="F143" s="3"/>
+      <c r="F143" s="3">
+        <v>19.273743</v>
+      </c>
       <c r="G143" s="5"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
@@ -5445,9 +5695,13 @@
       <c r="C144" t="s">
         <v>4</v>
       </c>
-      <c r="D144" s="3"/>
+      <c r="D144" s="3">
+        <v>12.975118999999999</v>
+      </c>
       <c r="E144" s="5"/>
-      <c r="F144" s="3"/>
+      <c r="F144" s="3">
+        <v>19.617785000000001</v>
+      </c>
       <c r="G144" s="5"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
@@ -5458,9 +5712,13 @@
       <c r="C145" t="s">
         <v>5</v>
       </c>
-      <c r="D145" s="3"/>
+      <c r="D145" s="3">
+        <v>10.810810999999999</v>
+      </c>
       <c r="E145" s="5"/>
-      <c r="F145" s="3"/>
+      <c r="F145" s="3">
+        <v>14.634145999999999</v>
+      </c>
       <c r="G145" s="5"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
@@ -5469,9 +5727,13 @@
       <c r="C146" t="s">
         <v>4</v>
       </c>
-      <c r="D146" s="3"/>
+      <c r="D146" s="3">
+        <v>12.971253000000001</v>
+      </c>
       <c r="E146" s="5"/>
-      <c r="F146" s="3"/>
+      <c r="F146" s="3">
+        <v>19.343686999999999</v>
+      </c>
       <c r="G146" s="5"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
@@ -5480,233 +5742,377 @@
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="1"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="4"/>
-      <c r="F147" s="2"/>
-      <c r="G147" s="4"/>
+      <c r="D147" s="2">
+        <v>712.61949700000002</v>
+      </c>
+      <c r="E147" s="4">
+        <v>1.0740000000000001E-3</v>
+      </c>
+      <c r="F147" s="2">
+        <v>2051.7028180000002</v>
+      </c>
+      <c r="G147" s="4">
+        <v>1.093E-3</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="18" t="s">
+      <c r="A148" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B148" s="19"/>
-      <c r="C148" s="19"/>
-      <c r="D148" s="20"/>
-      <c r="E148" s="20"/>
-      <c r="F148" s="19"/>
-      <c r="G148" s="21"/>
+      <c r="B148" s="24"/>
+      <c r="C148" s="24"/>
+      <c r="D148" s="23"/>
+      <c r="E148" s="23"/>
+      <c r="F148" s="24"/>
+      <c r="G148" s="25"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="25" t="s">
+      <c r="A149" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B149" s="31" t="s">
+      <c r="B149" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C149" s="32"/>
-      <c r="D149" s="29" t="s">
+      <c r="C149" s="17"/>
+      <c r="D149" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E149" s="30"/>
-      <c r="F149" s="29" t="s">
+      <c r="E149" s="29"/>
+      <c r="F149" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G149" s="30"/>
+      <c r="G149" s="29"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B150" s="15" t="s">
+      <c r="B150" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C150" s="17"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="6"/>
-      <c r="F150" s="7"/>
-      <c r="G150" s="6"/>
+      <c r="C150" s="45"/>
+      <c r="D150" s="33">
+        <v>4197.6031750000002</v>
+      </c>
+      <c r="E150" s="36">
+        <v>15.450535</v>
+      </c>
+      <c r="F150" s="33">
+        <v>4197.6031750000002</v>
+      </c>
+      <c r="G150" s="36">
+        <v>15.440269000000001</v>
+      </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="3"/>
-      <c r="B151" s="10" t="s">
+      <c r="A151" s="37"/>
+      <c r="B151" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C151" s="14"/>
-      <c r="D151" s="3"/>
-      <c r="E151" s="5"/>
-      <c r="F151" s="3"/>
-      <c r="G151" s="5"/>
+      <c r="C151" s="46"/>
+      <c r="D151" s="37">
+        <v>2876.6507940000001</v>
+      </c>
+      <c r="E151" s="40">
+        <v>12.653053</v>
+      </c>
+      <c r="F151" s="37">
+        <v>2876.6507940000001</v>
+      </c>
+      <c r="G151" s="40">
+        <v>12.676155</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="3"/>
-      <c r="B152" s="10" t="s">
+      <c r="A152" s="37"/>
+      <c r="B152" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C152" s="14"/>
-      <c r="D152" s="3"/>
-      <c r="E152" s="5"/>
-      <c r="F152" s="3"/>
-      <c r="G152" s="5"/>
+      <c r="C152" s="46"/>
+      <c r="D152" s="37">
+        <v>1290.619048</v>
+      </c>
+      <c r="E152" s="40">
+        <v>8.3028670000000009</v>
+      </c>
+      <c r="F152" s="37">
+        <v>1290.619048</v>
+      </c>
+      <c r="G152" s="40">
+        <v>8.3285789999999995</v>
+      </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" s="3"/>
-      <c r="B153" s="10" t="s">
+      <c r="A153" s="37"/>
+      <c r="B153" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C153" s="14"/>
-      <c r="D153" s="3"/>
-      <c r="E153" s="5"/>
-      <c r="F153" s="3"/>
-      <c r="G153" s="5"/>
+      <c r="C153" s="46"/>
+      <c r="D153" s="37">
+        <v>345.69841300000002</v>
+      </c>
+      <c r="E153" s="40">
+        <v>5.0313739999999996</v>
+      </c>
+      <c r="F153" s="37">
+        <v>345.69841300000002</v>
+      </c>
+      <c r="G153" s="40">
+        <v>5.0334070000000004</v>
+      </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B154" s="10" t="s">
+      <c r="B154" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C154" s="14"/>
-      <c r="D154" s="3"/>
-      <c r="E154" s="5"/>
-      <c r="F154" s="3"/>
-      <c r="G154" s="5"/>
+      <c r="C154" s="46"/>
+      <c r="D154" s="37">
+        <v>0</v>
+      </c>
+      <c r="E154" s="40">
+        <v>0</v>
+      </c>
+      <c r="F154" s="37">
+        <v>0</v>
+      </c>
+      <c r="G154" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A155" s="3"/>
-      <c r="B155" s="10" t="s">
+      <c r="A155" s="37"/>
+      <c r="B155" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C155" s="14"/>
-      <c r="D155" s="3"/>
-      <c r="E155" s="5"/>
-      <c r="F155" s="3"/>
-      <c r="G155" s="5"/>
+      <c r="C155" s="46"/>
+      <c r="D155" s="37">
+        <v>0</v>
+      </c>
+      <c r="E155" s="40">
+        <v>0</v>
+      </c>
+      <c r="F155" s="37">
+        <v>0</v>
+      </c>
+      <c r="G155" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A156" s="3"/>
-      <c r="B156" s="10" t="s">
+      <c r="A156" s="37"/>
+      <c r="B156" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C156" s="14"/>
-      <c r="D156" s="3"/>
-      <c r="E156" s="5"/>
-      <c r="F156" s="3"/>
-      <c r="G156" s="5"/>
+      <c r="C156" s="46"/>
+      <c r="D156" s="37">
+        <v>0</v>
+      </c>
+      <c r="E156" s="40">
+        <v>0</v>
+      </c>
+      <c r="F156" s="37">
+        <v>0</v>
+      </c>
+      <c r="G156" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A157" s="3"/>
-      <c r="B157" s="10" t="s">
+      <c r="A157" s="37"/>
+      <c r="B157" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C157" s="14"/>
-      <c r="D157" s="3"/>
-      <c r="E157" s="5"/>
-      <c r="F157" s="3"/>
-      <c r="G157" s="5"/>
+      <c r="C157" s="46"/>
+      <c r="D157" s="37">
+        <v>12.920635000000001</v>
+      </c>
+      <c r="E157" s="40">
+        <v>3.2192750000000001</v>
+      </c>
+      <c r="F157" s="37">
+        <v>12.698413</v>
+      </c>
+      <c r="G157" s="40">
+        <v>3.097267</v>
+      </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B158" s="10" t="s">
+      <c r="B158" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C158" s="14"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="5"/>
-      <c r="F158" s="3"/>
-      <c r="G158" s="5"/>
+      <c r="C158" s="46"/>
+      <c r="D158" s="37">
+        <v>1105.730159</v>
+      </c>
+      <c r="E158" s="40">
+        <v>7.3160400000000001</v>
+      </c>
+      <c r="F158" s="37">
+        <v>1105.730159</v>
+      </c>
+      <c r="G158" s="40">
+        <v>7.3145020000000001</v>
+      </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A159" s="3"/>
-      <c r="B159" s="10" t="s">
+      <c r="A159" s="37"/>
+      <c r="B159" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C159" s="14"/>
-      <c r="D159" s="3"/>
-      <c r="E159" s="5"/>
-      <c r="F159" s="3"/>
-      <c r="G159" s="5"/>
+      <c r="C159" s="46"/>
+      <c r="D159" s="37">
+        <v>752.84127000000001</v>
+      </c>
+      <c r="E159" s="40">
+        <v>6.5634959999999998</v>
+      </c>
+      <c r="F159" s="37">
+        <v>752.84127000000001</v>
+      </c>
+      <c r="G159" s="40">
+        <v>6.5619370000000004</v>
+      </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A160" s="3"/>
-      <c r="B160" s="10" t="s">
+      <c r="A160" s="37"/>
+      <c r="B160" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C160" s="14"/>
-      <c r="D160" s="3"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="3"/>
-      <c r="G160" s="5"/>
+      <c r="C160" s="46"/>
+      <c r="D160" s="37">
+        <v>338.49206299999997</v>
+      </c>
+      <c r="E160" s="40">
+        <v>4.4401849999999996</v>
+      </c>
+      <c r="F160" s="37">
+        <v>338.49206299999997</v>
+      </c>
+      <c r="G160" s="40">
+        <v>4.4408760000000003</v>
+      </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A161" s="3"/>
-      <c r="B161" s="10" t="s">
+      <c r="A161" s="37"/>
+      <c r="B161" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C161" s="14"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="5"/>
-      <c r="F161" s="3"/>
-      <c r="G161" s="5"/>
+      <c r="C161" s="46"/>
+      <c r="D161" s="37">
+        <v>86.380951999999994</v>
+      </c>
+      <c r="E161" s="40">
+        <v>2.7664080000000002</v>
+      </c>
+      <c r="F161" s="37">
+        <v>86.380951999999994</v>
+      </c>
+      <c r="G161" s="40">
+        <v>2.7664080000000002</v>
+      </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B162" s="10" t="s">
+      <c r="B162" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C162" s="14"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="5"/>
-      <c r="F162" s="3"/>
-      <c r="G162" s="5"/>
+      <c r="C162" s="46"/>
+      <c r="D162" s="37">
+        <v>3091.8412699999999</v>
+      </c>
+      <c r="E162" s="40">
+        <v>14.159535999999999</v>
+      </c>
+      <c r="F162" s="37">
+        <v>3091.8412699999999</v>
+      </c>
+      <c r="G162" s="40">
+        <v>14.190497000000001</v>
+      </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A163" s="3"/>
-      <c r="B163" s="10" t="s">
+      <c r="A163" s="37"/>
+      <c r="B163" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C163" s="14"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="5"/>
-      <c r="F163" s="3"/>
-      <c r="G163" s="5"/>
+      <c r="C163" s="46"/>
+      <c r="D163" s="37">
+        <v>2123.7619049999998</v>
+      </c>
+      <c r="E163" s="40">
+        <v>10.837126</v>
+      </c>
+      <c r="F163" s="37">
+        <v>2123.7619049999998</v>
+      </c>
+      <c r="G163" s="40">
+        <v>10.825414</v>
+      </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A164" s="3"/>
-      <c r="B164" s="10" t="s">
+      <c r="A164" s="37"/>
+      <c r="B164" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C164" s="14"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="5"/>
-      <c r="F164" s="3"/>
-      <c r="G164" s="5"/>
+      <c r="C164" s="46"/>
+      <c r="D164" s="37">
+        <v>952.063492</v>
+      </c>
+      <c r="E164" s="40">
+        <v>8.0875900000000005</v>
+      </c>
+      <c r="F164" s="37">
+        <v>952.063492</v>
+      </c>
+      <c r="G164" s="40">
+        <v>8.0882229999999993</v>
+      </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A165" s="3"/>
-      <c r="B165" s="10" t="s">
+      <c r="A165" s="37"/>
+      <c r="B165" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C165" s="14"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="5"/>
-      <c r="F165" s="3"/>
-      <c r="G165" s="5"/>
+      <c r="C165" s="46"/>
+      <c r="D165" s="37">
+        <v>239.12698399999999</v>
+      </c>
+      <c r="E165" s="40">
+        <v>3.8034729999999999</v>
+      </c>
+      <c r="F165" s="37">
+        <v>239.12698399999999</v>
+      </c>
+      <c r="G165" s="40">
+        <v>3.8034729999999999</v>
+      </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B166" s="2"/>
-      <c r="C166" s="4"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="4"/>
-      <c r="F166" s="2"/>
-      <c r="G166" s="4"/>
+      <c r="A166" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B166" s="41"/>
+      <c r="C166" s="44"/>
+      <c r="D166" s="41">
+        <v>249.18396799999999</v>
+      </c>
+      <c r="E166" s="44">
+        <v>31.213736000000001</v>
+      </c>
+      <c r="F166" s="41">
+        <v>249.31249199999999</v>
+      </c>
+      <c r="G166" s="44">
+        <v>31.124690000000001</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="50">
@@ -5720,6 +6126,12 @@
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="B104:C104"/>
     <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
     <mergeCell ref="D149:E149"/>
     <mergeCell ref="F149:G149"/>
     <mergeCell ref="A1:G1"/>
@@ -5736,12 +6148,6 @@
     <mergeCell ref="B99:C99"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
     <mergeCell ref="B112:C112"/>
     <mergeCell ref="B149:C149"/>
     <mergeCell ref="B150:C150"/>

</xml_diff>